<commit_message>
save as jsonl file update
</commit_message>
<xml_diff>
--- a/Test_Files.xlsx
+++ b/Test_Files.xlsx
@@ -601,7 +601,9 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>

</xml_diff>